<commit_message>
add linear reg code
</commit_message>
<xml_diff>
--- a/data/BFCN_t1_cov.xlsx
+++ b/data/BFCN_t1_cov.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suramericana.sharepoint.com/sites/Investigacin/Shared Documents/Proyectos/prisma/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jazmsure/Documents/PRISMA/prisma_pls/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7958F0C1-2BCC-41AA-982A-0BA0751EA21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D094C84C-7B40-3741-A513-8191189966E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2505,7 +2505,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2863,21 +2863,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CM200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="AZ1" sqref="AZ1:AZ1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="50" max="50" width="26" customWidth="1"/>
-    <col min="51" max="51" width="22.7109375" customWidth="1"/>
-    <col min="52" max="52" width="28.140625" customWidth="1"/>
-    <col min="53" max="53" width="25.140625" customWidth="1"/>
-    <col min="88" max="88" width="13.28515625" customWidth="1"/>
-    <col min="89" max="89" width="16.28515625" customWidth="1"/>
+    <col min="51" max="51" width="22.6640625" customWidth="1"/>
+    <col min="52" max="52" width="28.1640625" customWidth="1"/>
+    <col min="53" max="53" width="25.1640625" customWidth="1"/>
+    <col min="88" max="88" width="13.33203125" customWidth="1"/>
+    <col min="89" max="89" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91">
+    <row r="1" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3152,7 +3153,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:91">
+    <row r="2" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3415,7 +3416,7 @@
         <v>1518452.6</v>
       </c>
     </row>
-    <row r="3" spans="1:91">
+    <row r="3" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>104</v>
       </c>
@@ -3525,7 +3526,7 @@
         <v>1476873</v>
       </c>
     </row>
-    <row r="4" spans="1:91">
+    <row r="4" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -3641,7 +3642,7 @@
         <v>1421527.1</v>
       </c>
     </row>
-    <row r="5" spans="1:91">
+    <row r="5" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>1339354.8</v>
       </c>
     </row>
-    <row r="6" spans="1:91">
+    <row r="6" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>1386851.5</v>
       </c>
     </row>
-    <row r="7" spans="1:91">
+    <row r="7" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -4037,7 +4038,7 @@
         <v>1465279</v>
       </c>
     </row>
-    <row r="8" spans="1:91">
+    <row r="8" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -4153,7 +4154,7 @@
         <v>1388232.5</v>
       </c>
     </row>
-    <row r="9" spans="1:91">
+    <row r="9" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -4404,7 +4405,7 @@
         <v>1362039.6</v>
       </c>
     </row>
-    <row r="10" spans="1:91">
+    <row r="10" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4658,7 +4659,7 @@
         <v>1192530.2</v>
       </c>
     </row>
-    <row r="11" spans="1:91">
+    <row r="11" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -4909,7 +4910,7 @@
         <v>1396390.5</v>
       </c>
     </row>
-    <row r="12" spans="1:91">
+    <row r="12" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>1347423.2</v>
       </c>
     </row>
-    <row r="13" spans="1:91">
+    <row r="13" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -5261,7 +5262,7 @@
         <v>1569929</v>
       </c>
     </row>
-    <row r="14" spans="1:91">
+    <row r="14" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -5512,7 +5513,7 @@
         <v>1451514</v>
       </c>
     </row>
-    <row r="15" spans="1:91">
+    <row r="15" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -5760,7 +5761,7 @@
         <v>1284866.6000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:91">
+    <row r="16" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -6005,13 +6006,13 @@
         <v>4.5343743627804756</v>
       </c>
       <c r="CL16">
-        <v>64.640640258789063</v>
+        <v>64.640640258789062</v>
       </c>
       <c r="CM16">
         <v>1255362</v>
       </c>
     </row>
-    <row r="17" spans="1:91">
+    <row r="17" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>178</v>
       </c>
@@ -6253,13 +6254,13 @@
         <v>4.7342160599703211</v>
       </c>
       <c r="CL17">
-        <v>59.327285766601563</v>
+        <v>59.327285766601562</v>
       </c>
       <c r="CM17">
         <v>1507329.2</v>
       </c>
     </row>
-    <row r="18" spans="1:91">
+    <row r="18" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>1355595.4</v>
       </c>
     </row>
-    <row r="19" spans="1:91">
+    <row r="19" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -6479,7 +6480,7 @@
         <v>1484016.1</v>
       </c>
     </row>
-    <row r="20" spans="1:91">
+    <row r="20" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>188</v>
       </c>
@@ -6505,7 +6506,7 @@
         <v>1273660.3999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:91">
+    <row r="21" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -6759,7 +6760,7 @@
         <v>1700774.9</v>
       </c>
     </row>
-    <row r="22" spans="1:91">
+    <row r="22" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>1632945.6</v>
       </c>
     </row>
-    <row r="23" spans="1:91">
+    <row r="23" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>197</v>
       </c>
@@ -7120,7 +7121,7 @@
         <v>1288945.5</v>
       </c>
     </row>
-    <row r="24" spans="1:91">
+    <row r="24" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -7368,7 +7369,7 @@
         <v>1286930.1000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:91">
+    <row r="25" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>211</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>1610781.9</v>
       </c>
     </row>
-    <row r="26" spans="1:91">
+    <row r="26" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>216</v>
       </c>
@@ -7876,7 +7877,7 @@
         <v>1490988.9</v>
       </c>
     </row>
-    <row r="27" spans="1:91">
+    <row r="27" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -7989,7 +7990,7 @@
         <v>1621364.5</v>
       </c>
     </row>
-    <row r="28" spans="1:91">
+    <row r="28" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>223</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>1240835.6000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:91">
+    <row r="29" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>225</v>
       </c>
@@ -8356,7 +8357,7 @@
         <v>1304333.8</v>
       </c>
     </row>
-    <row r="30" spans="1:91">
+    <row r="30" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>234</v>
       </c>
@@ -8472,7 +8473,7 @@
         <v>1518343.4</v>
       </c>
     </row>
-    <row r="31" spans="1:91">
+    <row r="31" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>236</v>
       </c>
@@ -8723,7 +8724,7 @@
         <v>1306717.5</v>
       </c>
     </row>
-    <row r="32" spans="1:91">
+    <row r="32" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>242</v>
       </c>
@@ -8968,7 +8969,7 @@
         <v>1235764.1000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:91">
+    <row r="33" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>252</v>
       </c>
@@ -9204,7 +9205,7 @@
         <v>1637181.2</v>
       </c>
     </row>
-    <row r="34" spans="1:91">
+    <row r="34" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>255</v>
       </c>
@@ -9230,7 +9231,7 @@
         <v>1108583.6000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:91">
+    <row r="35" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>256</v>
       </c>
@@ -9346,7 +9347,7 @@
         <v>1740332.1</v>
       </c>
     </row>
-    <row r="36" spans="1:91">
+    <row r="36" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>258</v>
       </c>
@@ -9456,7 +9457,7 @@
         <v>1204642.5</v>
       </c>
     </row>
-    <row r="37" spans="1:91">
+    <row r="37" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>260</v>
       </c>
@@ -9569,7 +9570,7 @@
         <v>1754474.6</v>
       </c>
     </row>
-    <row r="38" spans="1:91">
+    <row r="38" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>262</v>
       </c>
@@ -9685,7 +9686,7 @@
         <v>1487164.2</v>
       </c>
     </row>
-    <row r="39" spans="1:91">
+    <row r="39" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>264</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>1227425.5</v>
       </c>
     </row>
-    <row r="40" spans="1:91">
+    <row r="40" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>266</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>1543868.6</v>
       </c>
     </row>
-    <row r="41" spans="1:91">
+    <row r="41" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>273</v>
       </c>
@@ -10312,7 +10313,7 @@
         <v>1192996.1000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:91">
+    <row r="42" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>282</v>
       </c>
@@ -10419,7 +10420,7 @@
         <v>9.2547321319580078</v>
       </c>
     </row>
-    <row r="43" spans="1:91">
+    <row r="43" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>284</v>
       </c>
@@ -10679,7 +10680,7 @@
         <v>23.896650314331051</v>
       </c>
     </row>
-    <row r="44" spans="1:91">
+    <row r="44" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>292</v>
       </c>
@@ -10930,7 +10931,7 @@
         <v>1487432.4</v>
       </c>
     </row>
-    <row r="45" spans="1:91">
+    <row r="45" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>300</v>
       </c>
@@ -11037,7 +11038,7 @@
         <v>31.28488731384277</v>
       </c>
     </row>
-    <row r="46" spans="1:91">
+    <row r="46" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>302</v>
       </c>
@@ -11153,7 +11154,7 @@
         <v>1466311.8</v>
       </c>
     </row>
-    <row r="47" spans="1:91">
+    <row r="47" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>304</v>
       </c>
@@ -11266,7 +11267,7 @@
         <v>1409378.1</v>
       </c>
     </row>
-    <row r="48" spans="1:91">
+    <row r="48" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>306</v>
       </c>
@@ -11514,7 +11515,7 @@
         <v>1327517.8999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:91">
+    <row r="49" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>311</v>
       </c>
@@ -11774,7 +11775,7 @@
         <v>1260992.6000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:91">
+    <row r="50" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>318</v>
       </c>
@@ -12025,7 +12026,7 @@
         <v>1509755</v>
       </c>
     </row>
-    <row r="51" spans="1:91">
+    <row r="51" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>326</v>
       </c>
@@ -12138,7 +12139,7 @@
         <v>1440520.8</v>
       </c>
     </row>
-    <row r="52" spans="1:91">
+    <row r="52" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>328</v>
       </c>
@@ -12389,7 +12390,7 @@
         <v>1237875.1000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:91">
+    <row r="53" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>336</v>
       </c>
@@ -12640,13 +12641,13 @@
         <v>4.688442946892085</v>
       </c>
       <c r="CL53">
-        <v>55.335464477539063</v>
+        <v>55.335464477539062</v>
       </c>
       <c r="CM53">
         <v>1500655.8</v>
       </c>
     </row>
-    <row r="54" spans="1:91">
+    <row r="54" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>341</v>
       </c>
@@ -12894,7 +12895,7 @@
         <v>1270850.8</v>
       </c>
     </row>
-    <row r="55" spans="1:91">
+    <row r="55" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>347</v>
       </c>
@@ -13139,7 +13140,7 @@
         <v>1441783.9</v>
       </c>
     </row>
-    <row r="56" spans="1:91">
+    <row r="56" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>354</v>
       </c>
@@ -13390,7 +13391,7 @@
         <v>1509287.8</v>
       </c>
     </row>
-    <row r="57" spans="1:91">
+    <row r="57" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>360</v>
       </c>
@@ -13644,7 +13645,7 @@
         <v>1259146</v>
       </c>
     </row>
-    <row r="58" spans="1:91">
+    <row r="58" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>366</v>
       </c>
@@ -13898,7 +13899,7 @@
         <v>1616456.4</v>
       </c>
     </row>
-    <row r="59" spans="1:91">
+    <row r="59" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>372</v>
       </c>
@@ -14011,7 +14012,7 @@
         <v>1500807.6</v>
       </c>
     </row>
-    <row r="60" spans="1:91">
+    <row r="60" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>374</v>
       </c>
@@ -14253,13 +14254,13 @@
         <v>3.602732256820361</v>
       </c>
       <c r="CL60">
-        <v>64.196487426757813</v>
+        <v>64.196487426757812</v>
       </c>
       <c r="CM60">
         <v>1530345.8</v>
       </c>
     </row>
-    <row r="61" spans="1:91">
+    <row r="61" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>380</v>
       </c>
@@ -14369,7 +14370,7 @@
         <v>1429796.5</v>
       </c>
     </row>
-    <row r="62" spans="1:91">
+    <row r="62" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>382</v>
       </c>
@@ -14479,7 +14480,7 @@
         <v>1412690.2</v>
       </c>
     </row>
-    <row r="63" spans="1:91">
+    <row r="63" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>384</v>
       </c>
@@ -14571,7 +14572,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:91">
+    <row r="64" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>386</v>
       </c>
@@ -14828,7 +14829,7 @@
         <v>906129.8</v>
       </c>
     </row>
-    <row r="65" spans="1:91">
+    <row r="65" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>393</v>
       </c>
@@ -14941,7 +14942,7 @@
         <v>1213297.8</v>
       </c>
     </row>
-    <row r="66" spans="1:91">
+    <row r="66" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>395</v>
       </c>
@@ -15195,7 +15196,7 @@
         <v>1101199.8999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:91">
+    <row r="67" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>402</v>
       </c>
@@ -15455,7 +15456,7 @@
         <v>1434280.2</v>
       </c>
     </row>
-    <row r="68" spans="1:91">
+    <row r="68" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>409</v>
       </c>
@@ -15703,7 +15704,7 @@
         <v>1371450.6</v>
       </c>
     </row>
-    <row r="69" spans="1:91">
+    <row r="69" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>415</v>
       </c>
@@ -15954,7 +15955,7 @@
         <v>1236843.5</v>
       </c>
     </row>
-    <row r="70" spans="1:91">
+    <row r="70" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>421</v>
       </c>
@@ -16205,7 +16206,7 @@
         <v>1182530.8</v>
       </c>
     </row>
-    <row r="71" spans="1:91">
+    <row r="71" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>425</v>
       </c>
@@ -16462,7 +16463,7 @@
         <v>1158208.8</v>
       </c>
     </row>
-    <row r="72" spans="1:91">
+    <row r="72" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>431</v>
       </c>
@@ -16572,7 +16573,7 @@
         <v>1186417</v>
       </c>
     </row>
-    <row r="73" spans="1:91">
+    <row r="73" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>433</v>
       </c>
@@ -16829,7 +16830,7 @@
         <v>1308666.8</v>
       </c>
     </row>
-    <row r="74" spans="1:91">
+    <row r="74" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>440</v>
       </c>
@@ -17086,7 +17087,7 @@
         <v>1295543.1000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:91">
+    <row r="75" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>447</v>
       </c>
@@ -17340,7 +17341,7 @@
         <v>1504579.8</v>
       </c>
     </row>
-    <row r="76" spans="1:91">
+    <row r="76" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>453</v>
       </c>
@@ -17591,7 +17592,7 @@
         <v>1276355.3999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:91">
+    <row r="77" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>458</v>
       </c>
@@ -17839,7 +17840,7 @@
         <v>1271948.2</v>
       </c>
     </row>
-    <row r="78" spans="1:91">
+    <row r="78" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>462</v>
       </c>
@@ -18087,13 +18088,13 @@
         <v>3.939553285304414</v>
       </c>
       <c r="CL78">
-        <v>42.504165649414063</v>
+        <v>42.504165649414062</v>
       </c>
       <c r="CM78">
         <v>1159261.8999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:91">
+    <row r="79" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>468</v>
       </c>
@@ -18350,7 +18351,7 @@
         <v>1384735.2</v>
       </c>
     </row>
-    <row r="80" spans="1:91">
+    <row r="80" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>473</v>
       </c>
@@ -18601,7 +18602,7 @@
         <v>1577508.1</v>
       </c>
     </row>
-    <row r="81" spans="1:91">
+    <row r="81" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>477</v>
       </c>
@@ -18858,7 +18859,7 @@
         <v>1226897.8999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:91">
+    <row r="82" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>483</v>
       </c>
@@ -19109,7 +19110,7 @@
         <v>1184233.1000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:91">
+    <row r="83" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>488</v>
       </c>
@@ -19366,7 +19367,7 @@
         <v>1532822.5</v>
       </c>
     </row>
-    <row r="84" spans="1:91">
+    <row r="84" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>493</v>
       </c>
@@ -19626,7 +19627,7 @@
         <v>1464172.2</v>
       </c>
     </row>
-    <row r="85" spans="1:91">
+    <row r="85" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>499</v>
       </c>
@@ -19874,7 +19875,7 @@
         <v>1189459.8</v>
       </c>
     </row>
-    <row r="86" spans="1:91">
+    <row r="86" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>502</v>
       </c>
@@ -20128,7 +20129,7 @@
         <v>1597007.8</v>
       </c>
     </row>
-    <row r="87" spans="1:91">
+    <row r="87" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>508</v>
       </c>
@@ -20382,7 +20383,7 @@
         <v>1294577.8</v>
       </c>
     </row>
-    <row r="88" spans="1:91">
+    <row r="88" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>514</v>
       </c>
@@ -20492,7 +20493,7 @@
         <v>1520144</v>
       </c>
     </row>
-    <row r="89" spans="1:91">
+    <row r="89" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>516</v>
       </c>
@@ -20758,7 +20759,7 @@
         <v>1344080.1</v>
       </c>
     </row>
-    <row r="90" spans="1:91">
+    <row r="90" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>522</v>
       </c>
@@ -21015,7 +21016,7 @@
         <v>1327311.1000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:91">
+    <row r="91" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>529</v>
       </c>
@@ -21257,7 +21258,7 @@
         <v>1513397.8</v>
       </c>
     </row>
-    <row r="92" spans="1:91">
+    <row r="92" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>532</v>
       </c>
@@ -21511,7 +21512,7 @@
         <v>1329459.8</v>
       </c>
     </row>
-    <row r="93" spans="1:91">
+    <row r="93" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>538</v>
       </c>
@@ -21762,7 +21763,7 @@
         <v>1364679.5</v>
       </c>
     </row>
-    <row r="94" spans="1:91">
+    <row r="94" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>542</v>
       </c>
@@ -22013,7 +22014,7 @@
         <v>1613103</v>
       </c>
     </row>
-    <row r="95" spans="1:91">
+    <row r="95" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>546</v>
       </c>
@@ -22270,7 +22271,7 @@
         <v>1575858.6</v>
       </c>
     </row>
-    <row r="96" spans="1:91">
+    <row r="96" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>551</v>
       </c>
@@ -22509,7 +22510,7 @@
         <v>1148595.6000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:91">
+    <row r="97" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>555</v>
       </c>
@@ -22625,7 +22626,7 @@
         <v>1376051.8</v>
       </c>
     </row>
-    <row r="98" spans="1:91">
+    <row r="98" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>557</v>
       </c>
@@ -22864,7 +22865,7 @@
         <v>1319820.3999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:91">
+    <row r="99" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>563</v>
       </c>
@@ -23109,7 +23110,7 @@
         <v>1480241.9</v>
       </c>
     </row>
-    <row r="100" spans="1:91">
+    <row r="100" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>568</v>
       </c>
@@ -23363,7 +23364,7 @@
         <v>1264156.8</v>
       </c>
     </row>
-    <row r="101" spans="1:91">
+    <row r="101" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>575</v>
       </c>
@@ -23473,7 +23474,7 @@
         <v>945438.56</v>
       </c>
     </row>
-    <row r="102" spans="1:91">
+    <row r="102" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>577</v>
       </c>
@@ -23583,7 +23584,7 @@
         <v>1263691.6000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:91">
+    <row r="103" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>579</v>
       </c>
@@ -23693,7 +23694,7 @@
         <v>1216514.8999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:91">
+    <row r="104" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>581</v>
       </c>
@@ -23935,7 +23936,7 @@
         <v>1371582.8</v>
       </c>
     </row>
-    <row r="105" spans="1:91">
+    <row r="105" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>586</v>
       </c>
@@ -24045,7 +24046,7 @@
         <v>1433006.9</v>
       </c>
     </row>
-    <row r="106" spans="1:91">
+    <row r="106" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>588</v>
       </c>
@@ -24281,7 +24282,7 @@
         <v>1152271.8</v>
       </c>
     </row>
-    <row r="107" spans="1:91">
+    <row r="107" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>593</v>
       </c>
@@ -24535,7 +24536,7 @@
         <v>1370590.5</v>
       </c>
     </row>
-    <row r="108" spans="1:91">
+    <row r="108" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>597</v>
       </c>
@@ -24645,7 +24646,7 @@
         <v>1170221.5</v>
       </c>
     </row>
-    <row r="109" spans="1:91">
+    <row r="109" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>599</v>
       </c>
@@ -24749,13 +24750,13 @@
         <v>4.0419254015289399</v>
       </c>
       <c r="CL109">
-        <v>38.832290649414063</v>
+        <v>38.832290649414062</v>
       </c>
       <c r="CM109">
         <v>1284334.1000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:91">
+    <row r="110" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>601</v>
       </c>
@@ -24865,7 +24866,7 @@
         <v>1450954.5</v>
       </c>
     </row>
-    <row r="111" spans="1:91">
+    <row r="111" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>603</v>
       </c>
@@ -25110,7 +25111,7 @@
         <v>1518311.5</v>
       </c>
     </row>
-    <row r="112" spans="1:91">
+    <row r="112" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>607</v>
       </c>
@@ -25349,13 +25350,13 @@
         <v>4.3838760337008509</v>
       </c>
       <c r="CL112">
-        <v>32.590896606445313</v>
+        <v>32.590896606445312</v>
       </c>
       <c r="CM112">
         <v>1588069.5</v>
       </c>
     </row>
-    <row r="113" spans="1:91">
+    <row r="113" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>610</v>
       </c>
@@ -25594,7 +25595,7 @@
         <v>1225363.8</v>
       </c>
     </row>
-    <row r="114" spans="1:91">
+    <row r="114" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>613</v>
       </c>
@@ -25653,7 +25654,7 @@
         <v>1534736.6</v>
       </c>
     </row>
-    <row r="115" spans="1:91">
+    <row r="115" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>615</v>
       </c>
@@ -25763,7 +25764,7 @@
         <v>1481215.5</v>
       </c>
     </row>
-    <row r="116" spans="1:91">
+    <row r="116" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>617</v>
       </c>
@@ -25873,7 +25874,7 @@
         <v>1738483.1</v>
       </c>
     </row>
-    <row r="117" spans="1:91">
+    <row r="117" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>619</v>
       </c>
@@ -26130,7 +26131,7 @@
         <v>1210013.6000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:91">
+    <row r="118" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>624</v>
       </c>
@@ -26390,7 +26391,7 @@
         <v>1306834.8999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:91">
+    <row r="119" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>627</v>
       </c>
@@ -26635,7 +26636,7 @@
         <v>1167820.3999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:91">
+    <row r="120" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>633</v>
       </c>
@@ -26892,7 +26893,7 @@
         <v>1542468.2</v>
       </c>
     </row>
-    <row r="121" spans="1:91">
+    <row r="121" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>637</v>
       </c>
@@ -27146,7 +27147,7 @@
         <v>1591221.6</v>
       </c>
     </row>
-    <row r="122" spans="1:91">
+    <row r="122" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>641</v>
       </c>
@@ -27403,7 +27404,7 @@
         <v>1241384.8999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:91">
+    <row r="123" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>646</v>
       </c>
@@ -27651,7 +27652,7 @@
         <v>1254659.6000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:91">
+    <row r="124" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>649</v>
       </c>
@@ -27896,7 +27897,7 @@
         <v>1534697.6</v>
       </c>
     </row>
-    <row r="125" spans="1:91">
+    <row r="125" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>652</v>
       </c>
@@ -28144,7 +28145,7 @@
         <v>1260869.8</v>
       </c>
     </row>
-    <row r="126" spans="1:91">
+    <row r="126" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>657</v>
       </c>
@@ -28398,7 +28399,7 @@
         <v>1618696.6</v>
       </c>
     </row>
-    <row r="127" spans="1:91">
+    <row r="127" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>661</v>
       </c>
@@ -28637,13 +28638,13 @@
         <v>4.2828904263331999</v>
       </c>
       <c r="CL127">
-        <v>33.946060180664063</v>
+        <v>33.946060180664062</v>
       </c>
       <c r="CM127">
         <v>1251740.8</v>
       </c>
     </row>
-    <row r="128" spans="1:91">
+    <row r="128" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>667</v>
       </c>
@@ -28753,7 +28754,7 @@
         <v>1130774.6000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:91">
+    <row r="129" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>669</v>
       </c>
@@ -29001,7 +29002,7 @@
         <v>1212999.2</v>
       </c>
     </row>
-    <row r="130" spans="1:91">
+    <row r="130" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>674</v>
       </c>
@@ -29240,7 +29241,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="131" spans="1:91">
+    <row r="131" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>679</v>
       </c>
@@ -29479,7 +29480,7 @@
         <v>1434678.8</v>
       </c>
     </row>
-    <row r="132" spans="1:91">
+    <row r="132" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>681</v>
       </c>
@@ -29733,7 +29734,7 @@
         <v>1476694.5</v>
       </c>
     </row>
-    <row r="133" spans="1:91">
+    <row r="133" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>686</v>
       </c>
@@ -29981,7 +29982,7 @@
         <v>1263662.2</v>
       </c>
     </row>
-    <row r="134" spans="1:91">
+    <row r="134" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>693</v>
       </c>
@@ -30232,7 +30233,7 @@
         <v>1187259.2</v>
       </c>
     </row>
-    <row r="135" spans="1:91">
+    <row r="135" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>701</v>
       </c>
@@ -30252,13 +30253,13 @@
         <v>4.759087364700469</v>
       </c>
       <c r="CL135">
-        <v>58.112808227539063</v>
+        <v>58.112808227539062</v>
       </c>
       <c r="CM135">
         <v>1232677.6000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:91">
+    <row r="136" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>702</v>
       </c>
@@ -30509,7 +30510,7 @@
         <v>1103323.3999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:91">
+    <row r="137" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>708</v>
       </c>
@@ -30754,7 +30755,7 @@
         <v>1167806.2</v>
       </c>
     </row>
-    <row r="138" spans="1:91">
+    <row r="138" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>713</v>
       </c>
@@ -30783,7 +30784,7 @@
         <v>1518735.9</v>
       </c>
     </row>
-    <row r="139" spans="1:91">
+    <row r="139" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>715</v>
       </c>
@@ -31043,7 +31044,7 @@
         <v>1506141.4</v>
       </c>
     </row>
-    <row r="140" spans="1:91">
+    <row r="140" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>722</v>
       </c>
@@ -31147,7 +31148,7 @@
         <v>1311166.3999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:91">
+    <row r="141" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>724</v>
       </c>
@@ -31395,7 +31396,7 @@
         <v>1351075.8</v>
       </c>
     </row>
-    <row r="142" spans="1:91">
+    <row r="142" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>728</v>
       </c>
@@ -31634,13 +31635,13 @@
         <v>3.920983498256859</v>
       </c>
       <c r="CL142">
-        <v>52.836502075195313</v>
+        <v>52.836502075195312</v>
       </c>
       <c r="CM142">
         <v>1549323.5</v>
       </c>
     </row>
-    <row r="143" spans="1:91">
+    <row r="143" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>734</v>
       </c>
@@ -31891,7 +31892,7 @@
         <v>1275340.8</v>
       </c>
     </row>
-    <row r="144" spans="1:91">
+    <row r="144" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>739</v>
       </c>
@@ -32004,7 +32005,7 @@
         <v>1221459.8999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:91">
+    <row r="145" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>741</v>
       </c>
@@ -32252,7 +32253,7 @@
         <v>1268720.3999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:91">
+    <row r="146" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>748</v>
       </c>
@@ -32497,7 +32498,7 @@
         <v>1460109.6</v>
       </c>
     </row>
-    <row r="147" spans="1:91">
+    <row r="147" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>754</v>
       </c>
@@ -32736,7 +32737,7 @@
         <v>1184770.1000000001</v>
       </c>
     </row>
-    <row r="148" spans="1:91">
+    <row r="148" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>757</v>
       </c>
@@ -32846,7 +32847,7 @@
         <v>1157721.8</v>
       </c>
     </row>
-    <row r="149" spans="1:91">
+    <row r="149" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>759</v>
       </c>
@@ -33082,7 +33083,7 @@
         <v>1346493.4</v>
       </c>
     </row>
-    <row r="150" spans="1:91">
+    <row r="150" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>762</v>
       </c>
@@ -33192,7 +33193,7 @@
         <v>1484949.1</v>
       </c>
     </row>
-    <row r="151" spans="1:91">
+    <row r="151" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>764</v>
       </c>
@@ -33287,7 +33288,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="152" spans="1:91">
+    <row r="152" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>766</v>
       </c>
@@ -33379,7 +33380,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="153" spans="1:91">
+    <row r="153" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>768</v>
       </c>
@@ -33474,7 +33475,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="154" spans="1:91">
+    <row r="154" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>770</v>
       </c>
@@ -33572,7 +33573,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="155" spans="1:91">
+    <row r="155" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>772</v>
       </c>
@@ -33670,7 +33671,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="156" spans="1:91">
+    <row r="156" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>774</v>
       </c>
@@ -33762,7 +33763,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" spans="1:91">
+    <row r="157" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>776</v>
       </c>
@@ -33854,7 +33855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:91">
+    <row r="158" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>778</v>
       </c>
@@ -33873,6 +33874,9 @@
       <c r="K158">
         <v>16</v>
       </c>
+      <c r="CF158">
+        <v>111</v>
+      </c>
       <c r="CH158">
         <v>0.40171401440037968</v>
       </c>
@@ -33892,7 +33896,7 @@
         <v>1366870.1</v>
       </c>
     </row>
-    <row r="159" spans="1:91">
+    <row r="159" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>780</v>
       </c>
@@ -33911,6 +33915,9 @@
       <c r="K159">
         <v>17</v>
       </c>
+      <c r="CF159">
+        <v>90</v>
+      </c>
       <c r="CH159">
         <v>0.3123077664676196</v>
       </c>
@@ -33930,7 +33937,7 @@
         <v>1347186.2</v>
       </c>
     </row>
-    <row r="160" spans="1:91">
+    <row r="160" spans="1:91" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>781</v>
       </c>
@@ -33949,6 +33956,9 @@
       <c r="K160">
         <v>16</v>
       </c>
+      <c r="CF160">
+        <v>111</v>
+      </c>
       <c r="CH160">
         <v>0.46817361052762368</v>
       </c>
@@ -33968,7 +33978,7 @@
         <v>1154759.8</v>
       </c>
     </row>
-    <row r="161" spans="2:91">
+    <row r="161" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>782</v>
       </c>
@@ -33987,6 +33997,9 @@
       <c r="K161">
         <v>16</v>
       </c>
+      <c r="CF161">
+        <v>112</v>
+      </c>
       <c r="CH161">
         <v>0.38107777778121388</v>
       </c>
@@ -34006,7 +34019,7 @@
         <v>1480834.8</v>
       </c>
     </row>
-    <row r="162" spans="2:91">
+    <row r="162" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>783</v>
       </c>
@@ -34025,6 +34038,9 @@
       <c r="K162">
         <v>11</v>
       </c>
+      <c r="CF162">
+        <v>81</v>
+      </c>
       <c r="CH162">
         <v>0.3317526598288722</v>
       </c>
@@ -34044,7 +34060,7 @@
         <v>1487138.9</v>
       </c>
     </row>
-    <row r="163" spans="2:91">
+    <row r="163" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>784</v>
       </c>
@@ -34063,6 +34079,9 @@
       <c r="K163">
         <v>13</v>
       </c>
+      <c r="CF163">
+        <v>84</v>
+      </c>
       <c r="CH163">
         <v>0.2228481170740737</v>
       </c>
@@ -34082,7 +34101,7 @@
         <v>1463643.1</v>
       </c>
     </row>
-    <row r="164" spans="2:91">
+    <row r="164" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>785</v>
       </c>
@@ -34120,7 +34139,7 @@
         <v>1319421.6000000001</v>
       </c>
     </row>
-    <row r="165" spans="2:91">
+    <row r="165" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>786</v>
       </c>
@@ -34139,6 +34158,9 @@
       <c r="K165">
         <v>14</v>
       </c>
+      <c r="CF165">
+        <v>86</v>
+      </c>
       <c r="CH165">
         <v>0.20336845161111</v>
       </c>
@@ -34158,7 +34180,7 @@
         <v>1156863.8</v>
       </c>
     </row>
-    <row r="166" spans="2:91">
+    <row r="166" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>787</v>
       </c>
@@ -34177,6 +34199,9 @@
       <c r="K166">
         <v>11</v>
       </c>
+      <c r="CF166">
+        <v>65</v>
+      </c>
       <c r="CH166">
         <v>0.2110146597627815</v>
       </c>
@@ -34196,7 +34221,7 @@
         <v>1181897.5</v>
       </c>
     </row>
-    <row r="167" spans="2:91">
+    <row r="167" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>788</v>
       </c>
@@ -34215,6 +34240,9 @@
       <c r="K167">
         <v>16</v>
       </c>
+      <c r="CF167">
+        <v>110</v>
+      </c>
       <c r="CH167">
         <v>0.30215039785305908</v>
       </c>
@@ -34234,7 +34262,7 @@
         <v>1423232.5</v>
       </c>
     </row>
-    <row r="168" spans="2:91">
+    <row r="168" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>789</v>
       </c>
@@ -34253,6 +34281,9 @@
       <c r="K168">
         <v>15</v>
       </c>
+      <c r="CF168">
+        <v>113</v>
+      </c>
       <c r="CH168">
         <v>0.23983332506434299</v>
       </c>
@@ -34272,7 +34303,7 @@
         <v>1362422.2</v>
       </c>
     </row>
-    <row r="169" spans="2:91">
+    <row r="169" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>790</v>
       </c>
@@ -34291,6 +34322,9 @@
       <c r="K169">
         <v>7</v>
       </c>
+      <c r="CF169">
+        <v>73</v>
+      </c>
       <c r="CH169">
         <v>0.27974908177215069</v>
       </c>
@@ -34310,7 +34344,7 @@
         <v>1431505.8</v>
       </c>
     </row>
-    <row r="170" spans="2:91">
+    <row r="170" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>791</v>
       </c>
@@ -34329,6 +34363,9 @@
       <c r="K170">
         <v>15</v>
       </c>
+      <c r="CF170">
+        <v>81</v>
+      </c>
       <c r="CH170">
         <v>0.46841911320696478</v>
       </c>
@@ -34348,7 +34385,7 @@
         <v>1247702.1000000001</v>
       </c>
     </row>
-    <row r="171" spans="2:91">
+    <row r="171" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>792</v>
       </c>
@@ -34386,7 +34423,7 @@
         <v>1492198.3999999999</v>
       </c>
     </row>
-    <row r="172" spans="2:91">
+    <row r="172" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>793</v>
       </c>
@@ -34405,6 +34442,9 @@
       <c r="K172">
         <v>14</v>
       </c>
+      <c r="CF172">
+        <v>66</v>
+      </c>
       <c r="CH172">
         <v>0.27865210393100248</v>
       </c>
@@ -34424,7 +34464,7 @@
         <v>1240883.8</v>
       </c>
     </row>
-    <row r="173" spans="2:91">
+    <row r="173" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>794</v>
       </c>
@@ -34443,6 +34483,9 @@
       <c r="K173">
         <v>16</v>
       </c>
+      <c r="CF173">
+        <v>91</v>
+      </c>
       <c r="CH173">
         <v>0.39868759308080348</v>
       </c>
@@ -34462,7 +34505,7 @@
         <v>1183750.8</v>
       </c>
     </row>
-    <row r="174" spans="2:91">
+    <row r="174" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>795</v>
       </c>
@@ -34481,6 +34524,9 @@
       <c r="K174">
         <v>14</v>
       </c>
+      <c r="CF174">
+        <v>103</v>
+      </c>
       <c r="CH174">
         <v>0.23409997252567941</v>
       </c>
@@ -34500,7 +34546,7 @@
         <v>1271720.2</v>
       </c>
     </row>
-    <row r="175" spans="2:91">
+    <row r="175" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>796</v>
       </c>
@@ -34519,6 +34565,9 @@
       <c r="K175">
         <v>12.5</v>
       </c>
+      <c r="CF175">
+        <v>79</v>
+      </c>
       <c r="CH175">
         <v>0.43517007824987541</v>
       </c>
@@ -34538,7 +34587,7 @@
         <v>1183665</v>
       </c>
     </row>
-    <row r="176" spans="2:91">
+    <row r="176" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>797</v>
       </c>
@@ -34557,6 +34606,9 @@
       <c r="K176">
         <v>16</v>
       </c>
+      <c r="CF176">
+        <v>99</v>
+      </c>
       <c r="CH176">
         <v>0.16379595958977169</v>
       </c>
@@ -34576,7 +34628,7 @@
         <v>1130276.6000000001</v>
       </c>
     </row>
-    <row r="177" spans="2:91">
+    <row r="177" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>798</v>
       </c>
@@ -34595,6 +34647,9 @@
       <c r="K177">
         <v>12.5</v>
       </c>
+      <c r="CF177">
+        <v>69</v>
+      </c>
       <c r="CH177">
         <v>0.36808642269549419</v>
       </c>
@@ -34614,7 +34669,7 @@
         <v>1168746.6000000001</v>
       </c>
     </row>
-    <row r="178" spans="2:91">
+    <row r="178" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>799</v>
       </c>
@@ -34633,6 +34688,9 @@
       <c r="K178">
         <v>16</v>
       </c>
+      <c r="CF178">
+        <v>96</v>
+      </c>
       <c r="CH178">
         <v>0.3428364918795585</v>
       </c>
@@ -34652,7 +34710,7 @@
         <v>1546552.6</v>
       </c>
     </row>
-    <row r="179" spans="2:91">
+    <row r="179" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>800</v>
       </c>
@@ -34671,6 +34729,9 @@
       <c r="K179">
         <v>13</v>
       </c>
+      <c r="CF179">
+        <v>88</v>
+      </c>
       <c r="CH179">
         <v>0.64718425383119305</v>
       </c>
@@ -34690,7 +34751,7 @@
         <v>1157509.6000000001</v>
       </c>
     </row>
-    <row r="180" spans="2:91">
+    <row r="180" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>801</v>
       </c>
@@ -34709,6 +34770,9 @@
       <c r="K180">
         <v>18</v>
       </c>
+      <c r="CF180">
+        <v>111</v>
+      </c>
       <c r="CH180">
         <v>0.2373864896177951</v>
       </c>
@@ -34728,7 +34792,7 @@
         <v>1389612.9</v>
       </c>
     </row>
-    <row r="181" spans="2:91">
+    <row r="181" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>802</v>
       </c>
@@ -34747,6 +34811,9 @@
       <c r="K181">
         <v>13</v>
       </c>
+      <c r="CF181">
+        <v>81</v>
+      </c>
       <c r="CH181">
         <v>0.3944945021585855</v>
       </c>
@@ -34766,7 +34833,7 @@
         <v>1323197.6000000001</v>
       </c>
     </row>
-    <row r="182" spans="2:91">
+    <row r="182" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>803</v>
       </c>
@@ -34785,6 +34852,9 @@
       <c r="K182">
         <v>11</v>
       </c>
+      <c r="CF182">
+        <v>106</v>
+      </c>
       <c r="CH182">
         <v>0.2205860605982381</v>
       </c>
@@ -34804,7 +34874,7 @@
         <v>1148165.1000000001</v>
       </c>
     </row>
-    <row r="183" spans="2:91">
+    <row r="183" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>804</v>
       </c>
@@ -34823,6 +34893,9 @@
       <c r="K183">
         <v>5</v>
       </c>
+      <c r="CF183">
+        <v>73</v>
+      </c>
       <c r="CH183">
         <v>0.2118345769927972</v>
       </c>
@@ -34836,13 +34909,13 @@
         <v>4.7215031833774468</v>
       </c>
       <c r="CL183">
-        <v>68.524551391601563</v>
+        <v>68.524551391601562</v>
       </c>
       <c r="CM183">
         <v>1348281.8</v>
       </c>
     </row>
-    <row r="184" spans="2:91">
+    <row r="184" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>805</v>
       </c>
@@ -34880,7 +34953,7 @@
         <v>1211005.2</v>
       </c>
     </row>
-    <row r="185" spans="2:91">
+    <row r="185" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>806</v>
       </c>
@@ -34899,6 +34972,9 @@
       <c r="K185">
         <v>16</v>
       </c>
+      <c r="CF185">
+        <v>99</v>
+      </c>
       <c r="CH185">
         <v>0.4390589683356661</v>
       </c>
@@ -34918,7 +34994,7 @@
         <v>1806596.9</v>
       </c>
     </row>
-    <row r="186" spans="2:91">
+    <row r="186" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>807</v>
       </c>
@@ -34937,6 +35013,9 @@
       <c r="K186">
         <v>11</v>
       </c>
+      <c r="CF186">
+        <v>100</v>
+      </c>
       <c r="CH186">
         <v>0.30588407881728258</v>
       </c>
@@ -34950,13 +35029,13 @@
         <v>4.5353309198322913</v>
       </c>
       <c r="CL186">
-        <v>58.176345825195313</v>
+        <v>58.176345825195312</v>
       </c>
       <c r="CM186">
         <v>1308788.1000000001</v>
       </c>
     </row>
-    <row r="187" spans="2:91">
+    <row r="187" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>808</v>
       </c>
@@ -34975,6 +35054,9 @@
       <c r="K187">
         <v>11</v>
       </c>
+      <c r="CF187">
+        <v>72</v>
+      </c>
       <c r="CH187">
         <v>0.4601800225128605</v>
       </c>
@@ -34994,7 +35076,7 @@
         <v>1265800.5</v>
       </c>
     </row>
-    <row r="188" spans="2:91">
+    <row r="188" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>809</v>
       </c>
@@ -35032,7 +35114,7 @@
         <v>1277405.2</v>
       </c>
     </row>
-    <row r="189" spans="2:91">
+    <row r="189" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>810</v>
       </c>
@@ -35051,6 +35133,9 @@
       <c r="K189">
         <v>16</v>
       </c>
+      <c r="CF189">
+        <v>91</v>
+      </c>
       <c r="CH189">
         <v>0.12500846552917419</v>
       </c>
@@ -35070,7 +35155,7 @@
         <v>1328589.3999999999</v>
       </c>
     </row>
-    <row r="190" spans="2:91">
+    <row r="190" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>811</v>
       </c>
@@ -35089,6 +35174,9 @@
       <c r="K190">
         <v>16</v>
       </c>
+      <c r="CF190">
+        <v>90</v>
+      </c>
       <c r="CH190">
         <v>0.1951068283959719</v>
       </c>
@@ -35108,7 +35196,7 @@
         <v>1268769.6000000001</v>
       </c>
     </row>
-    <row r="191" spans="2:91">
+    <row r="191" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>812</v>
       </c>
@@ -35127,6 +35215,9 @@
       <c r="K191">
         <v>16</v>
       </c>
+      <c r="CF191">
+        <v>97</v>
+      </c>
       <c r="CH191">
         <v>0.54070348726305295</v>
       </c>
@@ -35146,7 +35237,7 @@
         <v>1381003.2</v>
       </c>
     </row>
-    <row r="192" spans="2:91">
+    <row r="192" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>813</v>
       </c>
@@ -35184,7 +35275,7 @@
         <v>1459474.6</v>
       </c>
     </row>
-    <row r="193" spans="2:91">
+    <row r="193" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>814</v>
       </c>
@@ -35203,6 +35294,9 @@
       <c r="K193">
         <v>11</v>
       </c>
+      <c r="CF193">
+        <v>98</v>
+      </c>
       <c r="CH193">
         <v>0.31770350866501501</v>
       </c>
@@ -35222,7 +35316,7 @@
         <v>1245164.2</v>
       </c>
     </row>
-    <row r="194" spans="2:91">
+    <row r="194" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>815</v>
       </c>
@@ -35241,6 +35335,9 @@
       <c r="K194">
         <v>16</v>
       </c>
+      <c r="CF194">
+        <v>79</v>
+      </c>
       <c r="CH194">
         <v>0.22404382307088441</v>
       </c>
@@ -35260,7 +35357,7 @@
         <v>1320202.3999999999</v>
       </c>
     </row>
-    <row r="195" spans="2:91">
+    <row r="195" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>816</v>
       </c>
@@ -35279,6 +35376,9 @@
       <c r="K195">
         <v>16</v>
       </c>
+      <c r="CF195">
+        <v>103</v>
+      </c>
       <c r="CH195">
         <v>0.27005443346730418</v>
       </c>
@@ -35298,7 +35398,7 @@
         <v>1442935.2</v>
       </c>
     </row>
-    <row r="196" spans="2:91">
+    <row r="196" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>817</v>
       </c>
@@ -35317,6 +35417,9 @@
       <c r="K196">
         <v>15</v>
       </c>
+      <c r="CF196">
+        <v>104</v>
+      </c>
       <c r="CH196">
         <v>0.26083242509070298</v>
       </c>
@@ -35336,7 +35439,7 @@
         <v>1526218.5</v>
       </c>
     </row>
-    <row r="197" spans="2:91">
+    <row r="197" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>818</v>
       </c>
@@ -35374,7 +35477,7 @@
         <v>1272899.6000000001</v>
       </c>
     </row>
-    <row r="198" spans="2:91">
+    <row r="198" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>819</v>
       </c>
@@ -35406,7 +35509,7 @@
         <v>35.952384948730469</v>
       </c>
     </row>
-    <row r="199" spans="2:91">
+    <row r="199" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>820</v>
       </c>
@@ -35438,7 +35541,7 @@
         <v>14.52281475067139</v>
       </c>
     </row>
-    <row r="200" spans="2:91">
+    <row r="200" spans="2:91" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>821</v>
       </c>
@@ -35476,28 +35579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7751d00f-774d-495c-bfb5-3c8e0f86e2bb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="94d1e7f6-f4a5-4ba8-aeae-59c7cca7fe74" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007899E7AB490CAC4A82AE3DF258BF44DA" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5b1ec7a7e0133fb88df7fb7d107e0837">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7751d00f-774d-495c-bfb5-3c8e0f86e2bb" xmlns:ns3="94d1e7f6-f4a5-4ba8-aeae-59c7cca7fe74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cce05cdf983b4cd63ce9e4e5c9bd167" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -35751,14 +35832,64 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7751d00f-774d-495c-bfb5-3c8e0f86e2bb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="94d1e7f6-f4a5-4ba8-aeae-59c7cca7fe74" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{998A4C71-ADA0-426F-AF7F-CF9469068732}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBF1C5CD-197E-47F5-980E-D875C359A5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7751d00f-774d-495c-bfb5-3c8e0f86e2bb"/>
+    <ds:schemaRef ds:uri="94d1e7f6-f4a5-4ba8-aeae-59c7cca7fe74"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C09C5892-3166-4EFF-80CF-5380CBD9025D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{998A4C71-ADA0-426F-AF7F-CF9469068732}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7751d00f-774d-495c-bfb5-3c8e0f86e2bb"/>
+    <ds:schemaRef ds:uri="94d1e7f6-f4a5-4ba8-aeae-59c7cca7fe74"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBF1C5CD-197E-47F5-980E-D875C359A5E9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C09C5892-3166-4EFF-80CF-5380CBD9025D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>